<commit_message>
Official ridership figures and T test
</commit_message>
<xml_diff>
--- a/doc/excels/temporal.xlsx
+++ b/doc/excels/temporal.xlsx
@@ -110,17 +110,17 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11614866259695066"/>
-          <c:y val="3.8849611883620933E-2"/>
-          <c:w val="0.8632520864667198"/>
-          <c:h val="0.76125512679709373"/>
+          <c:x val="0.1181581109084841"/>
+          <c:y val="3.9790280452231604E-2"/>
+          <c:w val="0.86275709317109939"/>
+          <c:h val="0.69249750560840917"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -136,7 +136,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -206,49 +206,49 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.45132743362831801</c:v>
+                  <c:v>0.54867256637168105</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40707964601769903</c:v>
+                  <c:v>0.50442477876106195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37168141592920301</c:v>
+                  <c:v>0.42477876106194601</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36283185840707899</c:v>
+                  <c:v>0.35398230088495503</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33628318584070799</c:v>
+                  <c:v>0.28318584070796399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30088495575221202</c:v>
+                  <c:v>0.238938053097345</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29203539823008801</c:v>
+                  <c:v>0.212389380530973</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.29203539823008801</c:v>
+                  <c:v>0.17699115044247701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28318584070796399</c:v>
+                  <c:v>0.15044247787610601</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.28318584070796399</c:v>
+                  <c:v>0.123893805309734</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.28318584070796399</c:v>
+                  <c:v>7.9646017699115002E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27433628318584002</c:v>
+                  <c:v>7.9646017699115002E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27433628318584002</c:v>
+                  <c:v>7.9646017699115002E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.27433628318584002</c:v>
+                  <c:v>6.19469026548672E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.27433628318584002</c:v>
+                  <c:v>5.30973451327433E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,7 +256,94 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-874E-4364-8993-23F26E7F6BE1}"/>
+              <c16:uniqueId val="{00000000-9C73-41A6-A66E-A3F4E977E159}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>percent of transit systems with positive response from convergent point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.7699115044247701E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7699115044247701E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8495575221238902E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9C73-41A6-A66E-A3F4E977E159}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -269,11 +356,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1337871903"/>
-        <c:axId val="1337877311"/>
+        <c:axId val="1228624735"/>
+        <c:axId val="1228640127"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1337871903"/>
+        <c:axId val="1228624735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,13 +387,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Temporal lag from incubation</a:t>
+                  <a:t>Incubation Lag</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> period</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -314,8 +396,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.33803046388864311"/>
-              <c:y val="0.90665524965407696"/>
+              <c:x val="0.4357001531291893"/>
+              <c:y val="0.80901666952647866"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -384,7 +466,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1337877311"/>
+        <c:crossAx val="1228640127"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -392,10 +474,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1337877311"/>
+        <c:axId val="1228640127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.2"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -433,14 +516,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Ratio</a:t>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Ratio of systems with positive reposne interval </a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of cities with positive reposne interval </a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -448,8 +531,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.4981273408239701E-2"/>
-              <c:y val="9.3779589608036604E-2"/>
+              <c:x val="2.0819777367727131E-2"/>
+              <c:y val="9.7901660597510057E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -512,7 +595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1337871903"/>
+        <c:crossAx val="1228624735"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -524,6 +607,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0253188438247575E-2"/>
+          <c:y val="0.8749558000165234"/>
+          <c:w val="0.81030531292090424"/>
+          <c:h val="0.12366081358474258"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1121,20 +1245,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>404811</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1415,15 +1539,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1448,19 +1573,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C2" s="1">
-        <v>0.45132743362831801</v>
+        <v>0.54867256637168105</v>
       </c>
       <c r="D2">
         <v>113</v>
       </c>
       <c r="E2">
-        <v>111</v>
-      </c>
-      <c r="F2">
-        <v>0.98230088495575196</v>
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1.7699115044247701E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1468,19 +1593,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
-        <v>0.40707964601769903</v>
+        <v>0.50442477876106195</v>
       </c>
       <c r="D3">
         <v>113</v>
       </c>
       <c r="E3">
-        <v>110</v>
-      </c>
-      <c r="F3">
-        <v>0.97345132743362806</v>
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.7699115044247701E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1488,19 +1613,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1">
-        <v>0.37168141592920301</v>
+        <v>0.42477876106194601</v>
       </c>
       <c r="D4">
         <v>113</v>
       </c>
       <c r="E4">
-        <v>109</v>
-      </c>
-      <c r="F4">
-        <v>0.96460176991150404</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8.8495575221238902E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1508,19 +1633,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1">
-        <v>0.36283185840707899</v>
+        <v>0.35398230088495503</v>
       </c>
       <c r="D5">
         <v>113</v>
       </c>
       <c r="E5">
-        <v>109</v>
-      </c>
-      <c r="F5">
-        <v>0.96460176991150404</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1528,19 +1653,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>0.33628318584070799</v>
+        <v>0.28318584070796399</v>
       </c>
       <c r="D6">
         <v>113</v>
       </c>
       <c r="E6">
-        <v>108</v>
-      </c>
-      <c r="F6">
-        <v>0.95575221238938002</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1548,19 +1673,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>0.30088495575221202</v>
+        <v>0.238938053097345</v>
       </c>
       <c r="D7">
         <v>113</v>
       </c>
       <c r="E7">
-        <v>108</v>
-      </c>
-      <c r="F7">
-        <v>0.95575221238938002</v>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1568,19 +1693,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
-        <v>0.29203539823008801</v>
+        <v>0.212389380530973</v>
       </c>
       <c r="D8">
         <v>113</v>
       </c>
       <c r="E8">
-        <v>107</v>
-      </c>
-      <c r="F8">
-        <v>0.946902654867256</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1588,19 +1713,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>0.29203539823008801</v>
+        <v>0.17699115044247701</v>
       </c>
       <c r="D9">
         <v>113</v>
       </c>
       <c r="E9">
-        <v>105</v>
-      </c>
-      <c r="F9">
-        <v>0.92920353982300796</v>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,19 +1733,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1">
-        <v>0.28318584070796399</v>
+        <v>0.15044247787610601</v>
       </c>
       <c r="D10">
         <v>113</v>
       </c>
       <c r="E10">
-        <v>104</v>
-      </c>
-      <c r="F10">
-        <v>0.92035398230088405</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1628,19 +1753,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
-        <v>0.28318584070796399</v>
+        <v>0.123893805309734</v>
       </c>
       <c r="D11">
         <v>113</v>
       </c>
       <c r="E11">
-        <v>98</v>
-      </c>
-      <c r="F11">
-        <v>0.86725663716814105</v>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1648,19 +1773,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>0.28318584070796399</v>
+        <v>7.9646017699115002E-2</v>
       </c>
       <c r="D12">
         <v>113</v>
       </c>
       <c r="E12">
-        <v>97</v>
-      </c>
-      <c r="F12">
-        <v>0.85840707964601703</v>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1668,19 +1793,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>0.27433628318584002</v>
+        <v>7.9646017699115002E-2</v>
       </c>
       <c r="D13">
         <v>113</v>
       </c>
       <c r="E13">
-        <v>91</v>
-      </c>
-      <c r="F13">
-        <v>0.80530973451327403</v>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1688,19 +1813,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>0.27433628318584002</v>
+        <v>7.9646017699115002E-2</v>
       </c>
       <c r="D14">
         <v>113</v>
       </c>
       <c r="E14">
-        <v>87</v>
-      </c>
-      <c r="F14">
-        <v>0.76991150442477796</v>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1708,19 +1833,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>0.27433628318584002</v>
+        <v>6.19469026548672E-2</v>
       </c>
       <c r="D15">
         <v>113</v>
       </c>
       <c r="E15">
-        <v>79</v>
-      </c>
-      <c r="F15">
-        <v>0.69911504424778703</v>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1728,19 +1853,139 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
-        <v>0.27433628318584002</v>
+        <v>5.30973451327433E-2</v>
       </c>
       <c r="D16">
         <v>113</v>
       </c>
       <c r="E16">
-        <v>74</v>
-      </c>
-      <c r="F16">
-        <v>0.65486725663716805</v>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="C33" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update new correlation results
</commit_message>
<xml_diff>
--- a/doc/excels/temporal.xlsx
+++ b/doc/excels/temporal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="incubation_lag" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$C$114</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4353,7 +4352,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5323,7 +5321,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11128,8 +11125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11888,6 +11885,24 @@
       <c r="I26">
         <f t="shared" si="0"/>
         <v>-0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>C26-B26</f>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="D27">
+        <f>E26-D26</f>
+        <v>-0.625</v>
+      </c>
+      <c r="F27">
+        <f>G26-F26</f>
+        <v>-0.58333333333333326</v>
+      </c>
+      <c r="H27">
+        <f>I26-H26</f>
+        <v>0.70833333333333326</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -22237,7 +22252,7 @@
         <v>2</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M97" si="3">L66-K66</f>
+        <f t="shared" ref="M66:M94" si="3">L66-K66</f>
         <v>0</v>
       </c>
     </row>
@@ -47499,7 +47514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update more draft and almost finish the first draft. Need to do: create a collective curve plot; and update new hourly data; and refine the peak analysis.
</commit_message>
<xml_diff>
--- a/doc/excels/temporal.xlsx
+++ b/doc/excels/temporal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="incubation_lag" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="392">
   <si>
     <t># transit systems with positive response from divergent point</t>
   </si>
@@ -1201,6 +1201,18 @@
   <si>
     <t># Total posts</t>
   </si>
+  <si>
+    <t>NZ_morning_shift</t>
+  </si>
+  <si>
+    <t>NZ_afternoon_shift</t>
+  </si>
+  <si>
+    <t>AU_morning_shift</t>
+  </si>
+  <si>
+    <t>AU_afternoon_shift</t>
+  </si>
 </sst>
 </file>
 
@@ -4270,7 +4282,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11123,15 +11134,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>377</v>
       </c>
@@ -11156,8 +11167,20 @@
       <c r="I1" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>388</v>
+      </c>
+      <c r="K1" t="s">
+        <v>389</v>
+      </c>
+      <c r="L1" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20200316</v>
       </c>
@@ -11185,8 +11208,20 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20200317</v>
       </c>
@@ -11214,8 +11249,20 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>-1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20200318</v>
       </c>
@@ -11243,8 +11290,20 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>-1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20200319</v>
       </c>
@@ -11272,8 +11331,20 @@
       <c r="I5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20200320</v>
       </c>
@@ -11301,8 +11372,20 @@
       <c r="I6">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20200323</v>
       </c>
@@ -11330,8 +11413,20 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20200324</v>
       </c>
@@ -11359,8 +11454,20 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20200325</v>
       </c>
@@ -11388,8 +11495,20 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>-3</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20200326</v>
       </c>
@@ -11417,8 +11536,20 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20200327</v>
       </c>
@@ -11446,8 +11577,20 @@
       <c r="I11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20200330</v>
       </c>
@@ -11475,8 +11618,20 @@
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20200331</v>
       </c>
@@ -11504,8 +11659,20 @@
       <c r="I13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20200401</v>
       </c>
@@ -11533,8 +11700,20 @@
       <c r="I14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>-2</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20200402</v>
       </c>
@@ -11562,8 +11741,20 @@
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20200403</v>
       </c>
@@ -11591,8 +11782,20 @@
       <c r="I16">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>-1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20200406</v>
       </c>
@@ -11620,8 +11823,20 @@
       <c r="I17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>20200407</v>
       </c>
@@ -11649,8 +11864,20 @@
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20200408</v>
       </c>
@@ -11678,8 +11905,20 @@
       <c r="I19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20200409</v>
       </c>
@@ -11707,8 +11946,20 @@
       <c r="I20">
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>-1</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20200410</v>
       </c>
@@ -11736,8 +11987,20 @@
       <c r="I21">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20200413</v>
       </c>
@@ -11765,8 +12028,20 @@
       <c r="I22">
         <v>-1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>-4</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20200414</v>
       </c>
@@ -11794,8 +12069,20 @@
       <c r="I23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>-4</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20200415</v>
       </c>
@@ -11823,8 +12110,20 @@
       <c r="I24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>-2</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20200416</v>
       </c>
@@ -11852,97 +12151,145 @@
       <c r="I25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>-3</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20200417</v>
+      </c>
       <c r="B26">
-        <f>AVERAGE(B2:B25)</f>
-        <v>-1.0416666666666667</v>
+        <v>-5</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:I26" si="0">AVERAGE(C2:C25)</f>
-        <v>0.29166666666666669</v>
+        <v>-2</v>
       </c>
       <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>-2</v>
+      </c>
+      <c r="G26">
+        <v>-1</v>
+      </c>
+      <c r="H26">
+        <v>-1</v>
+      </c>
+      <c r="I26">
+        <v>-1</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>AVERAGE(B2:B26)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:M27" si="0">AVERAGE(C2:C26)</f>
+        <v>0.2</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="0"/>
-        <v>-0.125</v>
-      </c>
-      <c r="E26">
+        <v>-0.12</v>
+      </c>
+      <c r="E27">
         <f t="shared" si="0"/>
-        <v>-0.75</v>
-      </c>
-      <c r="F26">
+        <v>-0.72</v>
+      </c>
+      <c r="F27">
         <f t="shared" si="0"/>
-        <v>-1.7083333333333333</v>
-      </c>
-      <c r="G26">
+        <v>-1.72</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="0"/>
-        <v>-2.2916666666666665</v>
-      </c>
-      <c r="H26">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="0"/>
-        <v>-1.125</v>
-      </c>
-      <c r="I26">
+        <v>-1.1200000000000001</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="0"/>
-        <v>-0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <f>C26-B26</f>
-        <v>1.3333333333333335</v>
-      </c>
-      <c r="D27">
-        <f>E26-D26</f>
-        <v>-0.625</v>
-      </c>
-      <c r="F27">
-        <f>G26-F26</f>
-        <v>-0.58333333333333326</v>
-      </c>
-      <c r="H27">
-        <f>I26-H26</f>
-        <v>0.70833333333333326</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30">
+        <v>-0.44</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>1.24</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="0"/>
+        <v>-0.52</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="0"/>
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f>C27-B27</f>
+        <v>1.4</v>
+      </c>
+      <c r="D28">
+        <f>E27-D27</f>
+        <v>-0.6</v>
+      </c>
+      <c r="F28">
+        <f>G27-F27</f>
+        <v>-0.52000000000000024</v>
+      </c>
+      <c r="H28">
+        <f>I27-H27</f>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="J28">
+        <f>K27-J27</f>
+        <v>-1.76</v>
+      </c>
+      <c r="L28">
+        <f>M27-L27</f>
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>20200321</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>-3</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>3</v>
-      </c>
-      <c r="D30">
-        <v>-1</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>-2</v>
-      </c>
-      <c r="G30">
-        <v>-6</v>
-      </c>
-      <c r="H30">
-        <v>-1</v>
-      </c>
-      <c r="I30">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>20200322</v>
-      </c>
-      <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
       </c>
       <c r="D31">
         <v>-1</v>
@@ -11954,7 +12301,7 @@
         <v>-2</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="H31">
         <v>-1</v>
@@ -11962,16 +12309,28 @@
       <c r="I31">
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>-1</v>
+      </c>
+      <c r="K31">
+        <v>-2</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>20200328</v>
+        <v>20200322</v>
       </c>
       <c r="B32">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="D32">
         <v>-1</v>
@@ -11983,7 +12342,7 @@
         <v>-2</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>-1</v>
@@ -11991,16 +12350,28 @@
       <c r="I32">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>-1</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>20200329</v>
+        <v>20200328</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="D33">
         <v>-1</v>
@@ -12012,24 +12383,36 @@
         <v>-2</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H33">
         <v>-1</v>
       </c>
       <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="J33">
+        <v>-1</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>20200404</v>
+        <v>20200329</v>
       </c>
       <c r="B34">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34">
         <v>-1</v>
@@ -12041,24 +12424,36 @@
         <v>-2</v>
       </c>
       <c r="G34">
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <v>-1</v>
       </c>
       <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>20200405</v>
+        <v>20200404</v>
       </c>
       <c r="B35">
         <v>-3</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>-1</v>
@@ -12070,27 +12465,39 @@
         <v>-2</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="H35">
         <v>-1</v>
       </c>
       <c r="I35">
+        <v>-1</v>
+      </c>
+      <c r="J35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>20200411</v>
+        <v>20200405</v>
       </c>
       <c r="B36">
+        <v>-3</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
         <v>-1</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -12099,7 +12506,7 @@
         <v>-2</v>
       </c>
       <c r="G36">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>-1</v>
@@ -12107,16 +12514,28 @@
       <c r="I36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>-6</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>20200412</v>
+        <v>20200411</v>
       </c>
       <c r="B37">
         <v>-1</v>
       </c>
       <c r="C37">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -12128,7 +12547,7 @@
         <v>-2</v>
       </c>
       <c r="G37">
-        <v>5</v>
+        <v>-3</v>
       </c>
       <c r="H37">
         <v>-1</v>
@@ -12136,16 +12555,28 @@
       <c r="I37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>3</v>
+      </c>
+      <c r="M37">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>20200417</v>
+        <v>20200412</v>
       </c>
       <c r="B38">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="C38">
-        <v>-2</v>
+        <v>8</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -12157,16 +12588,28 @@
         <v>-2</v>
       </c>
       <c r="G38">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="H38">
         <v>-1</v>
       </c>
       <c r="I38">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>-3</v>
+      </c>
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>20200418</v>
       </c>
@@ -12193,6 +12636,18 @@
       </c>
       <c r="I39">
         <v>0</v>
+      </c>
+      <c r="J39">
+        <v>-1</v>
+      </c>
+      <c r="K39">
+        <v>-3</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update several graphs (peak, average procrustes with error bar, new peak shift cartographic works), new peak analysis until May 10th, update semi-first draft.
</commit_message>
<xml_diff>
--- a/doc/excels/temporal.xlsx
+++ b/doc/excels/temporal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="incubation_lag" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,14 @@
     <sheet name="distance_sensitivity" sheetId="8" r:id="rId8"/>
     <sheet name="shift" sheetId="9" r:id="rId9"/>
     <sheet name="countries_peak_shift" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId11"/>
+    <sheet name="countries_peak_shift_2" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId12"/>
+    <sheet name="daily_average_procrustes_distan" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">correlation_of_floor_value!$A$1:$H$114</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">hourly_first_day!$H$1:$M$94</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Sheet2!$A$1:$D$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Sheet2!$A$1:$D$114</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet3!$A$1:$B$1048569</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet4!$A$1:$C$114</definedName>
   </definedNames>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="399">
   <si>
     <t># transit systems with positive response from divergent point</t>
   </si>
@@ -1213,15 +1215,49 @@
   <si>
     <t>AU_afternoon_shift</t>
   </si>
+  <si>
+    <t>Procrustes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United Kingdom </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United States </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> France </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Canada </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> New Zealand </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Australia </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1247,12 +1283,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4363,6 +4401,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5332,6 +5371,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11136,8 +11176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12656,6 +12696,3034 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:X42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20200316</v>
+      </c>
+      <c r="B2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>20200316</v>
+      </c>
+      <c r="F2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>20200316</v>
+      </c>
+      <c r="J2" t="s">
+        <v>395</v>
+      </c>
+      <c r="K2">
+        <v>-2</v>
+      </c>
+      <c r="L2">
+        <v>-1</v>
+      </c>
+      <c r="M2">
+        <v>20200316</v>
+      </c>
+      <c r="N2" t="s">
+        <v>396</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>20200316</v>
+      </c>
+      <c r="R2" t="s">
+        <v>397</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>20200316</v>
+      </c>
+      <c r="V2" t="s">
+        <v>398</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20200317</v>
+      </c>
+      <c r="B3" t="s">
+        <v>393</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>20200317</v>
+      </c>
+      <c r="F3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <v>20200317</v>
+      </c>
+      <c r="J3" t="s">
+        <v>395</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>20200317</v>
+      </c>
+      <c r="N3" t="s">
+        <v>396</v>
+      </c>
+      <c r="O3">
+        <v>-1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>20200317</v>
+      </c>
+      <c r="R3" t="s">
+        <v>397</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>20200317</v>
+      </c>
+      <c r="V3" t="s">
+        <v>398</v>
+      </c>
+      <c r="W3">
+        <v>-1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>20200318</v>
+      </c>
+      <c r="B4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-1</v>
+      </c>
+      <c r="E4">
+        <v>20200318</v>
+      </c>
+      <c r="F4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>20200318</v>
+      </c>
+      <c r="J4" t="s">
+        <v>395</v>
+      </c>
+      <c r="K4">
+        <v>-1</v>
+      </c>
+      <c r="L4">
+        <v>-3</v>
+      </c>
+      <c r="M4">
+        <v>20200318</v>
+      </c>
+      <c r="N4" t="s">
+        <v>396</v>
+      </c>
+      <c r="O4">
+        <v>-1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>20200318</v>
+      </c>
+      <c r="R4" t="s">
+        <v>397</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>20200318</v>
+      </c>
+      <c r="V4" t="s">
+        <v>398</v>
+      </c>
+      <c r="W4">
+        <v>-1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20200319</v>
+      </c>
+      <c r="B5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>20200319</v>
+      </c>
+      <c r="F5" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>20200319</v>
+      </c>
+      <c r="J5" t="s">
+        <v>395</v>
+      </c>
+      <c r="K5">
+        <v>-2</v>
+      </c>
+      <c r="L5">
+        <v>-5</v>
+      </c>
+      <c r="M5">
+        <v>20200319</v>
+      </c>
+      <c r="N5" t="s">
+        <v>396</v>
+      </c>
+      <c r="O5">
+        <v>-1</v>
+      </c>
+      <c r="P5">
+        <v>-1</v>
+      </c>
+      <c r="Q5">
+        <v>20200319</v>
+      </c>
+      <c r="R5" t="s">
+        <v>397</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>20200319</v>
+      </c>
+      <c r="V5" t="s">
+        <v>398</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20200320</v>
+      </c>
+      <c r="B6" t="s">
+        <v>393</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>20200320</v>
+      </c>
+      <c r="F6" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>20200320</v>
+      </c>
+      <c r="J6" t="s">
+        <v>395</v>
+      </c>
+      <c r="K6">
+        <v>-2</v>
+      </c>
+      <c r="L6">
+        <v>-3</v>
+      </c>
+      <c r="M6">
+        <v>20200320</v>
+      </c>
+      <c r="N6" t="s">
+        <v>396</v>
+      </c>
+      <c r="O6">
+        <v>-1</v>
+      </c>
+      <c r="P6">
+        <v>-1</v>
+      </c>
+      <c r="Q6">
+        <v>20200320</v>
+      </c>
+      <c r="R6" t="s">
+        <v>397</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>20200320</v>
+      </c>
+      <c r="V6" t="s">
+        <v>398</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20200323</v>
+      </c>
+      <c r="B7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>20200323</v>
+      </c>
+      <c r="F7" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>20200323</v>
+      </c>
+      <c r="J7" t="s">
+        <v>395</v>
+      </c>
+      <c r="K7">
+        <v>-2</v>
+      </c>
+      <c r="L7">
+        <v>-3</v>
+      </c>
+      <c r="M7">
+        <v>20200323</v>
+      </c>
+      <c r="N7" t="s">
+        <v>396</v>
+      </c>
+      <c r="O7">
+        <v>-1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>20200323</v>
+      </c>
+      <c r="R7" t="s">
+        <v>397</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>20200323</v>
+      </c>
+      <c r="V7" t="s">
+        <v>398</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20200324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-5</v>
+      </c>
+      <c r="E8">
+        <v>20200324</v>
+      </c>
+      <c r="F8" t="s">
+        <v>394</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>20200324</v>
+      </c>
+      <c r="J8" t="s">
+        <v>395</v>
+      </c>
+      <c r="K8">
+        <v>-2</v>
+      </c>
+      <c r="L8">
+        <v>-3</v>
+      </c>
+      <c r="M8">
+        <v>20200324</v>
+      </c>
+      <c r="N8" t="s">
+        <v>396</v>
+      </c>
+      <c r="O8">
+        <v>-1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>20200324</v>
+      </c>
+      <c r="R8" t="s">
+        <v>397</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>20200324</v>
+      </c>
+      <c r="V8" t="s">
+        <v>398</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20200325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>20200325</v>
+      </c>
+      <c r="F9" t="s">
+        <v>394</v>
+      </c>
+      <c r="G9">
+        <v>-1</v>
+      </c>
+      <c r="H9">
+        <v>-1</v>
+      </c>
+      <c r="I9">
+        <v>20200325</v>
+      </c>
+      <c r="J9" t="s">
+        <v>395</v>
+      </c>
+      <c r="K9">
+        <v>-2</v>
+      </c>
+      <c r="L9">
+        <v>-5</v>
+      </c>
+      <c r="M9">
+        <v>20200325</v>
+      </c>
+      <c r="N9" t="s">
+        <v>396</v>
+      </c>
+      <c r="O9">
+        <v>-1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>20200325</v>
+      </c>
+      <c r="R9" t="s">
+        <v>397</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>-3</v>
+      </c>
+      <c r="U9">
+        <v>20200325</v>
+      </c>
+      <c r="V9" t="s">
+        <v>398</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20200326</v>
+      </c>
+      <c r="B10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>20200326</v>
+      </c>
+      <c r="F10" t="s">
+        <v>394</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>20200326</v>
+      </c>
+      <c r="J10" t="s">
+        <v>395</v>
+      </c>
+      <c r="K10">
+        <v>-2</v>
+      </c>
+      <c r="L10">
+        <v>-1</v>
+      </c>
+      <c r="M10">
+        <v>20200326</v>
+      </c>
+      <c r="N10" t="s">
+        <v>396</v>
+      </c>
+      <c r="O10">
+        <v>-1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>20200326</v>
+      </c>
+      <c r="R10" t="s">
+        <v>397</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>20200326</v>
+      </c>
+      <c r="V10" t="s">
+        <v>398</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20200327</v>
+      </c>
+      <c r="B11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11">
+        <v>-1</v>
+      </c>
+      <c r="D11">
+        <v>-1</v>
+      </c>
+      <c r="E11">
+        <v>20200327</v>
+      </c>
+      <c r="F11" t="s">
+        <v>394</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>20200327</v>
+      </c>
+      <c r="J11" t="s">
+        <v>395</v>
+      </c>
+      <c r="K11">
+        <v>-2</v>
+      </c>
+      <c r="L11">
+        <v>-2</v>
+      </c>
+      <c r="M11">
+        <v>20200327</v>
+      </c>
+      <c r="N11" t="s">
+        <v>396</v>
+      </c>
+      <c r="O11">
+        <v>-1</v>
+      </c>
+      <c r="P11">
+        <v>-1</v>
+      </c>
+      <c r="Q11">
+        <v>20200327</v>
+      </c>
+      <c r="R11" t="s">
+        <v>397</v>
+      </c>
+      <c r="S11">
+        <v>4</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>20200327</v>
+      </c>
+      <c r="V11" t="s">
+        <v>398</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20200330</v>
+      </c>
+      <c r="B12" t="s">
+        <v>393</v>
+      </c>
+      <c r="C12">
+        <v>-1</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>20200330</v>
+      </c>
+      <c r="F12" t="s">
+        <v>394</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>-1</v>
+      </c>
+      <c r="I12">
+        <v>20200330</v>
+      </c>
+      <c r="J12" t="s">
+        <v>395</v>
+      </c>
+      <c r="K12">
+        <v>-2</v>
+      </c>
+      <c r="L12">
+        <v>-3</v>
+      </c>
+      <c r="M12">
+        <v>20200330</v>
+      </c>
+      <c r="N12" t="s">
+        <v>396</v>
+      </c>
+      <c r="O12">
+        <v>-1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>20200330</v>
+      </c>
+      <c r="R12" t="s">
+        <v>397</v>
+      </c>
+      <c r="S12">
+        <v>2</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>20200330</v>
+      </c>
+      <c r="V12" t="s">
+        <v>398</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20200331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>20200331</v>
+      </c>
+      <c r="F13" t="s">
+        <v>394</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>-1</v>
+      </c>
+      <c r="I13">
+        <v>20200331</v>
+      </c>
+      <c r="J13" t="s">
+        <v>395</v>
+      </c>
+      <c r="K13">
+        <v>-2</v>
+      </c>
+      <c r="L13">
+        <v>-3</v>
+      </c>
+      <c r="M13">
+        <v>20200331</v>
+      </c>
+      <c r="N13" t="s">
+        <v>396</v>
+      </c>
+      <c r="O13">
+        <v>-1</v>
+      </c>
+      <c r="P13">
+        <v>-1</v>
+      </c>
+      <c r="Q13">
+        <v>20200331</v>
+      </c>
+      <c r="R13" t="s">
+        <v>397</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>20200331</v>
+      </c>
+      <c r="V13" t="s">
+        <v>398</v>
+      </c>
+      <c r="W13">
+        <v>3</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20200401</v>
+      </c>
+      <c r="B14" t="s">
+        <v>393</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>20200401</v>
+      </c>
+      <c r="F14" t="s">
+        <v>394</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>-1</v>
+      </c>
+      <c r="I14">
+        <v>20200401</v>
+      </c>
+      <c r="J14" t="s">
+        <v>395</v>
+      </c>
+      <c r="K14">
+        <v>-2</v>
+      </c>
+      <c r="L14">
+        <v>-2</v>
+      </c>
+      <c r="M14">
+        <v>20200401</v>
+      </c>
+      <c r="N14" t="s">
+        <v>396</v>
+      </c>
+      <c r="O14">
+        <v>-2</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>20200401</v>
+      </c>
+      <c r="R14" t="s">
+        <v>397</v>
+      </c>
+      <c r="S14">
+        <v>4</v>
+      </c>
+      <c r="T14">
+        <v>-2</v>
+      </c>
+      <c r="U14">
+        <v>20200401</v>
+      </c>
+      <c r="V14" t="s">
+        <v>398</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20200402</v>
+      </c>
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+      <c r="C15">
+        <v>-1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>20200402</v>
+      </c>
+      <c r="F15" t="s">
+        <v>394</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>20200402</v>
+      </c>
+      <c r="J15" t="s">
+        <v>395</v>
+      </c>
+      <c r="K15">
+        <v>-2</v>
+      </c>
+      <c r="L15">
+        <v>-1</v>
+      </c>
+      <c r="M15">
+        <v>20200402</v>
+      </c>
+      <c r="N15" t="s">
+        <v>396</v>
+      </c>
+      <c r="O15">
+        <v>-1</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>20200402</v>
+      </c>
+      <c r="R15" t="s">
+        <v>397</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>20200402</v>
+      </c>
+      <c r="V15" t="s">
+        <v>398</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20200403</v>
+      </c>
+      <c r="B16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16">
+        <v>-1</v>
+      </c>
+      <c r="D16">
+        <v>-3</v>
+      </c>
+      <c r="E16">
+        <v>20200403</v>
+      </c>
+      <c r="F16" t="s">
+        <v>394</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>20200403</v>
+      </c>
+      <c r="J16" t="s">
+        <v>395</v>
+      </c>
+      <c r="K16">
+        <v>-2</v>
+      </c>
+      <c r="L16">
+        <v>-2</v>
+      </c>
+      <c r="M16">
+        <v>20200403</v>
+      </c>
+      <c r="N16" t="s">
+        <v>396</v>
+      </c>
+      <c r="O16">
+        <v>-1</v>
+      </c>
+      <c r="P16">
+        <v>-1</v>
+      </c>
+      <c r="Q16">
+        <v>20200403</v>
+      </c>
+      <c r="R16" t="s">
+        <v>397</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>-1</v>
+      </c>
+      <c r="U16">
+        <v>20200403</v>
+      </c>
+      <c r="V16" t="s">
+        <v>398</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20200406</v>
+      </c>
+      <c r="B17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C17">
+        <v>-4</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>20200406</v>
+      </c>
+      <c r="F17" t="s">
+        <v>394</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>20200406</v>
+      </c>
+      <c r="J17" t="s">
+        <v>395</v>
+      </c>
+      <c r="K17">
+        <v>-2</v>
+      </c>
+      <c r="L17">
+        <v>-4</v>
+      </c>
+      <c r="M17">
+        <v>20200406</v>
+      </c>
+      <c r="N17" t="s">
+        <v>396</v>
+      </c>
+      <c r="O17">
+        <v>-2</v>
+      </c>
+      <c r="P17">
+        <v>-1</v>
+      </c>
+      <c r="Q17">
+        <v>20200406</v>
+      </c>
+      <c r="R17" t="s">
+        <v>397</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>20200406</v>
+      </c>
+      <c r="V17" t="s">
+        <v>398</v>
+      </c>
+      <c r="W17">
+        <v>2</v>
+      </c>
+      <c r="X17">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20200407</v>
+      </c>
+      <c r="B18" t="s">
+        <v>393</v>
+      </c>
+      <c r="C18">
+        <v>-5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>20200407</v>
+      </c>
+      <c r="F18" t="s">
+        <v>394</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>-1</v>
+      </c>
+      <c r="I18">
+        <v>20200407</v>
+      </c>
+      <c r="J18" t="s">
+        <v>395</v>
+      </c>
+      <c r="K18">
+        <v>-2</v>
+      </c>
+      <c r="L18">
+        <v>-2</v>
+      </c>
+      <c r="M18">
+        <v>20200407</v>
+      </c>
+      <c r="N18" t="s">
+        <v>396</v>
+      </c>
+      <c r="O18">
+        <v>-2</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>20200407</v>
+      </c>
+      <c r="R18" t="s">
+        <v>397</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>20200407</v>
+      </c>
+      <c r="V18" t="s">
+        <v>398</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20200408</v>
+      </c>
+      <c r="B19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C19">
+        <v>-4</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>20200408</v>
+      </c>
+      <c r="F19" t="s">
+        <v>394</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>-2</v>
+      </c>
+      <c r="I19">
+        <v>20200408</v>
+      </c>
+      <c r="J19" t="s">
+        <v>395</v>
+      </c>
+      <c r="K19">
+        <v>-2</v>
+      </c>
+      <c r="L19">
+        <v>-2</v>
+      </c>
+      <c r="M19">
+        <v>20200408</v>
+      </c>
+      <c r="N19" t="s">
+        <v>396</v>
+      </c>
+      <c r="O19">
+        <v>-1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>20200408</v>
+      </c>
+      <c r="R19" t="s">
+        <v>397</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>20200408</v>
+      </c>
+      <c r="V19" t="s">
+        <v>398</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20200409</v>
+      </c>
+      <c r="B20" t="s">
+        <v>393</v>
+      </c>
+      <c r="C20">
+        <v>-2</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>20200409</v>
+      </c>
+      <c r="F20" t="s">
+        <v>394</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>-1</v>
+      </c>
+      <c r="I20">
+        <v>20200409</v>
+      </c>
+      <c r="J20" t="s">
+        <v>395</v>
+      </c>
+      <c r="K20">
+        <v>-2</v>
+      </c>
+      <c r="L20">
+        <v>-2</v>
+      </c>
+      <c r="M20">
+        <v>20200409</v>
+      </c>
+      <c r="N20" t="s">
+        <v>396</v>
+      </c>
+      <c r="O20">
+        <v>-1</v>
+      </c>
+      <c r="P20">
+        <v>-1</v>
+      </c>
+      <c r="Q20">
+        <v>20200409</v>
+      </c>
+      <c r="R20" t="s">
+        <v>397</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+      <c r="T20">
+        <v>-1</v>
+      </c>
+      <c r="U20">
+        <v>20200409</v>
+      </c>
+      <c r="V20" t="s">
+        <v>398</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20200410</v>
+      </c>
+      <c r="B21" t="s">
+        <v>393</v>
+      </c>
+      <c r="C21">
+        <v>-1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>20200410</v>
+      </c>
+      <c r="F21" t="s">
+        <v>394</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>20200410</v>
+      </c>
+      <c r="J21" t="s">
+        <v>395</v>
+      </c>
+      <c r="K21">
+        <v>-2</v>
+      </c>
+      <c r="L21">
+        <v>-3</v>
+      </c>
+      <c r="M21">
+        <v>20200410</v>
+      </c>
+      <c r="N21" t="s">
+        <v>396</v>
+      </c>
+      <c r="O21">
+        <v>-1</v>
+      </c>
+      <c r="P21">
+        <v>-1</v>
+      </c>
+      <c r="Q21">
+        <v>20200410</v>
+      </c>
+      <c r="R21" t="s">
+        <v>397</v>
+      </c>
+      <c r="S21">
+        <v>2</v>
+      </c>
+      <c r="T21">
+        <v>2</v>
+      </c>
+      <c r="U21">
+        <v>20200410</v>
+      </c>
+      <c r="V21" t="s">
+        <v>398</v>
+      </c>
+      <c r="W21">
+        <v>3</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20200413</v>
+      </c>
+      <c r="B22" t="s">
+        <v>393</v>
+      </c>
+      <c r="C22">
+        <v>-1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>20200413</v>
+      </c>
+      <c r="F22" t="s">
+        <v>394</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>-1</v>
+      </c>
+      <c r="I22">
+        <v>20200413</v>
+      </c>
+      <c r="J22" t="s">
+        <v>395</v>
+      </c>
+      <c r="K22">
+        <v>-1</v>
+      </c>
+      <c r="L22">
+        <v>-3</v>
+      </c>
+      <c r="M22">
+        <v>20200413</v>
+      </c>
+      <c r="N22" t="s">
+        <v>396</v>
+      </c>
+      <c r="O22">
+        <v>-2</v>
+      </c>
+      <c r="P22">
+        <v>-1</v>
+      </c>
+      <c r="Q22">
+        <v>20200413</v>
+      </c>
+      <c r="R22" t="s">
+        <v>397</v>
+      </c>
+      <c r="S22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>-4</v>
+      </c>
+      <c r="U22">
+        <v>20200413</v>
+      </c>
+      <c r="V22" t="s">
+        <v>398</v>
+      </c>
+      <c r="W22">
+        <v>2</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20200414</v>
+      </c>
+      <c r="B23" t="s">
+        <v>393</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>20200414</v>
+      </c>
+      <c r="F23" t="s">
+        <v>394</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>-1</v>
+      </c>
+      <c r="I23">
+        <v>20200414</v>
+      </c>
+      <c r="J23" t="s">
+        <v>395</v>
+      </c>
+      <c r="K23">
+        <v>-2</v>
+      </c>
+      <c r="L23">
+        <v>-1</v>
+      </c>
+      <c r="M23">
+        <v>20200414</v>
+      </c>
+      <c r="N23" t="s">
+        <v>396</v>
+      </c>
+      <c r="O23">
+        <v>-2</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>20200414</v>
+      </c>
+      <c r="R23" t="s">
+        <v>397</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>-4</v>
+      </c>
+      <c r="U23">
+        <v>20200414</v>
+      </c>
+      <c r="V23" t="s">
+        <v>398</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="X23">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20200415</v>
+      </c>
+      <c r="B24" t="s">
+        <v>393</v>
+      </c>
+      <c r="C24">
+        <v>-2</v>
+      </c>
+      <c r="D24">
+        <v>-1</v>
+      </c>
+      <c r="E24">
+        <v>20200415</v>
+      </c>
+      <c r="F24" t="s">
+        <v>394</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>-2</v>
+      </c>
+      <c r="I24">
+        <v>20200415</v>
+      </c>
+      <c r="J24" t="s">
+        <v>395</v>
+      </c>
+      <c r="K24">
+        <v>-2</v>
+      </c>
+      <c r="L24">
+        <v>-2</v>
+      </c>
+      <c r="M24">
+        <v>20200415</v>
+      </c>
+      <c r="N24" t="s">
+        <v>396</v>
+      </c>
+      <c r="O24">
+        <v>-1</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>20200415</v>
+      </c>
+      <c r="R24" t="s">
+        <v>397</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>-2</v>
+      </c>
+      <c r="U24">
+        <v>20200415</v>
+      </c>
+      <c r="V24" t="s">
+        <v>398</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20200416</v>
+      </c>
+      <c r="B25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C25">
+        <v>-2</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>20200416</v>
+      </c>
+      <c r="F25" t="s">
+        <v>394</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>-1</v>
+      </c>
+      <c r="I25">
+        <v>20200416</v>
+      </c>
+      <c r="J25" t="s">
+        <v>395</v>
+      </c>
+      <c r="K25">
+        <v>-2</v>
+      </c>
+      <c r="L25">
+        <v>-1</v>
+      </c>
+      <c r="M25">
+        <v>20200416</v>
+      </c>
+      <c r="N25" t="s">
+        <v>396</v>
+      </c>
+      <c r="O25">
+        <v>-1</v>
+      </c>
+      <c r="P25">
+        <v>-1</v>
+      </c>
+      <c r="Q25">
+        <v>20200416</v>
+      </c>
+      <c r="R25" t="s">
+        <v>397</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
+      <c r="T25">
+        <v>-3</v>
+      </c>
+      <c r="U25">
+        <v>20200416</v>
+      </c>
+      <c r="V25" t="s">
+        <v>398</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20200417</v>
+      </c>
+      <c r="B26" t="s">
+        <v>393</v>
+      </c>
+      <c r="C26">
+        <v>-5</v>
+      </c>
+      <c r="D26">
+        <v>-2</v>
+      </c>
+      <c r="E26">
+        <v>20200417</v>
+      </c>
+      <c r="F26" t="s">
+        <v>394</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>20200417</v>
+      </c>
+      <c r="J26" t="s">
+        <v>395</v>
+      </c>
+      <c r="K26">
+        <v>-2</v>
+      </c>
+      <c r="L26">
+        <v>-1</v>
+      </c>
+      <c r="M26">
+        <v>20200417</v>
+      </c>
+      <c r="N26" t="s">
+        <v>396</v>
+      </c>
+      <c r="O26">
+        <v>-1</v>
+      </c>
+      <c r="P26">
+        <v>-1</v>
+      </c>
+      <c r="Q26">
+        <v>20200417</v>
+      </c>
+      <c r="R26" t="s">
+        <v>397</v>
+      </c>
+      <c r="S26">
+        <v>4</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>20200417</v>
+      </c>
+      <c r="V26" t="s">
+        <v>398</v>
+      </c>
+      <c r="W26">
+        <v>3</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20200420</v>
+      </c>
+      <c r="B27" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27">
+        <v>-5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>20200420</v>
+      </c>
+      <c r="F27" t="s">
+        <v>394</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>20200420</v>
+      </c>
+      <c r="J27" t="s">
+        <v>395</v>
+      </c>
+      <c r="K27">
+        <v>-2</v>
+      </c>
+      <c r="L27">
+        <v>-2</v>
+      </c>
+      <c r="M27">
+        <v>20200420</v>
+      </c>
+      <c r="N27" t="s">
+        <v>396</v>
+      </c>
+      <c r="O27">
+        <v>-1</v>
+      </c>
+      <c r="P27">
+        <v>-1</v>
+      </c>
+      <c r="Q27">
+        <v>20200420</v>
+      </c>
+      <c r="R27" t="s">
+        <v>397</v>
+      </c>
+      <c r="S27">
+        <v>-1</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>20200420</v>
+      </c>
+      <c r="V27" t="s">
+        <v>398</v>
+      </c>
+      <c r="W27">
+        <v>3</v>
+      </c>
+      <c r="X27">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20200421</v>
+      </c>
+      <c r="B28" t="s">
+        <v>393</v>
+      </c>
+      <c r="C28">
+        <v>-1</v>
+      </c>
+      <c r="D28">
+        <v>-5</v>
+      </c>
+      <c r="E28">
+        <v>20200421</v>
+      </c>
+      <c r="F28" t="s">
+        <v>394</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>-1</v>
+      </c>
+      <c r="I28">
+        <v>20200421</v>
+      </c>
+      <c r="J28" t="s">
+        <v>395</v>
+      </c>
+      <c r="K28">
+        <v>-2</v>
+      </c>
+      <c r="L28">
+        <v>-2</v>
+      </c>
+      <c r="M28">
+        <v>20200421</v>
+      </c>
+      <c r="N28" t="s">
+        <v>396</v>
+      </c>
+      <c r="O28">
+        <v>-2</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>20200421</v>
+      </c>
+      <c r="R28" t="s">
+        <v>397</v>
+      </c>
+      <c r="S28">
+        <v>3</v>
+      </c>
+      <c r="T28">
+        <v>-1</v>
+      </c>
+      <c r="U28">
+        <v>20200421</v>
+      </c>
+      <c r="V28" t="s">
+        <v>398</v>
+      </c>
+      <c r="W28">
+        <v>3</v>
+      </c>
+      <c r="X28">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20200422</v>
+      </c>
+      <c r="B29" t="s">
+        <v>393</v>
+      </c>
+      <c r="C29">
+        <v>-1</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>20200422</v>
+      </c>
+      <c r="F29" t="s">
+        <v>394</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>-2</v>
+      </c>
+      <c r="I29">
+        <v>20200422</v>
+      </c>
+      <c r="J29" t="s">
+        <v>395</v>
+      </c>
+      <c r="K29">
+        <v>-2</v>
+      </c>
+      <c r="L29">
+        <v>-1</v>
+      </c>
+      <c r="M29">
+        <v>20200422</v>
+      </c>
+      <c r="N29" t="s">
+        <v>396</v>
+      </c>
+      <c r="O29">
+        <v>-1</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>20200422</v>
+      </c>
+      <c r="R29" t="s">
+        <v>397</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>-1</v>
+      </c>
+      <c r="U29">
+        <v>20200422</v>
+      </c>
+      <c r="V29" t="s">
+        <v>398</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20200423</v>
+      </c>
+      <c r="B30" t="s">
+        <v>393</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>20200423</v>
+      </c>
+      <c r="F30" t="s">
+        <v>394</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>20200423</v>
+      </c>
+      <c r="J30" t="s">
+        <v>395</v>
+      </c>
+      <c r="K30">
+        <v>-2</v>
+      </c>
+      <c r="L30">
+        <v>-2</v>
+      </c>
+      <c r="M30">
+        <v>20200423</v>
+      </c>
+      <c r="N30" t="s">
+        <v>396</v>
+      </c>
+      <c r="O30">
+        <v>-1</v>
+      </c>
+      <c r="P30">
+        <v>-1</v>
+      </c>
+      <c r="Q30">
+        <v>20200423</v>
+      </c>
+      <c r="R30" t="s">
+        <v>397</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>20200423</v>
+      </c>
+      <c r="V30" t="s">
+        <v>398</v>
+      </c>
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20200424</v>
+      </c>
+      <c r="B31" t="s">
+        <v>393</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>20200424</v>
+      </c>
+      <c r="F31" t="s">
+        <v>394</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>20200424</v>
+      </c>
+      <c r="J31" t="s">
+        <v>395</v>
+      </c>
+      <c r="K31">
+        <v>-2</v>
+      </c>
+      <c r="L31">
+        <v>-1</v>
+      </c>
+      <c r="M31">
+        <v>20200424</v>
+      </c>
+      <c r="N31" t="s">
+        <v>396</v>
+      </c>
+      <c r="O31">
+        <v>-1</v>
+      </c>
+      <c r="P31">
+        <v>-1</v>
+      </c>
+      <c r="Q31">
+        <v>20200424</v>
+      </c>
+      <c r="R31" t="s">
+        <v>397</v>
+      </c>
+      <c r="S31">
+        <v>4</v>
+      </c>
+      <c r="T31">
+        <v>2</v>
+      </c>
+      <c r="U31">
+        <v>20200424</v>
+      </c>
+      <c r="V31" t="s">
+        <v>398</v>
+      </c>
+      <c r="W31">
+        <v>2</v>
+      </c>
+      <c r="X31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20200427</v>
+      </c>
+      <c r="B32" t="s">
+        <v>393</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>-1</v>
+      </c>
+      <c r="E32">
+        <v>20200427</v>
+      </c>
+      <c r="F32" t="s">
+        <v>394</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>20200427</v>
+      </c>
+      <c r="J32" t="s">
+        <v>395</v>
+      </c>
+      <c r="K32">
+        <v>-2</v>
+      </c>
+      <c r="L32">
+        <v>-1</v>
+      </c>
+      <c r="M32">
+        <v>20200427</v>
+      </c>
+      <c r="N32" t="s">
+        <v>396</v>
+      </c>
+      <c r="O32">
+        <v>-1</v>
+      </c>
+      <c r="P32">
+        <v>-1</v>
+      </c>
+      <c r="Q32">
+        <v>20200427</v>
+      </c>
+      <c r="R32" t="s">
+        <v>397</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>20200427</v>
+      </c>
+      <c r="V32" t="s">
+        <v>398</v>
+      </c>
+      <c r="W32">
+        <v>-1</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20200428</v>
+      </c>
+      <c r="B33" t="s">
+        <v>393</v>
+      </c>
+      <c r="C33">
+        <v>-1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>20200428</v>
+      </c>
+      <c r="F33" t="s">
+        <v>394</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>-1</v>
+      </c>
+      <c r="I33">
+        <v>20200428</v>
+      </c>
+      <c r="J33" t="s">
+        <v>395</v>
+      </c>
+      <c r="K33">
+        <v>-2</v>
+      </c>
+      <c r="L33">
+        <v>-1</v>
+      </c>
+      <c r="M33">
+        <v>20200428</v>
+      </c>
+      <c r="N33" t="s">
+        <v>396</v>
+      </c>
+      <c r="O33">
+        <v>-2</v>
+      </c>
+      <c r="P33">
+        <v>-1</v>
+      </c>
+      <c r="Q33">
+        <v>20200428</v>
+      </c>
+      <c r="R33" t="s">
+        <v>397</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>-1</v>
+      </c>
+      <c r="U33">
+        <v>20200428</v>
+      </c>
+      <c r="V33" t="s">
+        <v>398</v>
+      </c>
+      <c r="W33">
+        <v>2</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>20200429</v>
+      </c>
+      <c r="B34" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>20200429</v>
+      </c>
+      <c r="F34" t="s">
+        <v>394</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>20200429</v>
+      </c>
+      <c r="J34" t="s">
+        <v>395</v>
+      </c>
+      <c r="K34">
+        <v>-2</v>
+      </c>
+      <c r="L34">
+        <v>-1</v>
+      </c>
+      <c r="M34">
+        <v>20200429</v>
+      </c>
+      <c r="N34" t="s">
+        <v>396</v>
+      </c>
+      <c r="O34">
+        <v>-2</v>
+      </c>
+      <c r="P34">
+        <v>-1</v>
+      </c>
+      <c r="Q34">
+        <v>20200429</v>
+      </c>
+      <c r="R34" t="s">
+        <v>397</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>20200429</v>
+      </c>
+      <c r="V34" t="s">
+        <v>398</v>
+      </c>
+      <c r="W34">
+        <v>-1</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>20200430</v>
+      </c>
+      <c r="B35" t="s">
+        <v>393</v>
+      </c>
+      <c r="C35">
+        <v>-2</v>
+      </c>
+      <c r="D35">
+        <v>-3</v>
+      </c>
+      <c r="E35">
+        <v>20200430</v>
+      </c>
+      <c r="F35" t="s">
+        <v>394</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>-1</v>
+      </c>
+      <c r="I35">
+        <v>20200430</v>
+      </c>
+      <c r="J35" t="s">
+        <v>395</v>
+      </c>
+      <c r="K35">
+        <v>-2</v>
+      </c>
+      <c r="L35">
+        <v>-2</v>
+      </c>
+      <c r="M35">
+        <v>20200430</v>
+      </c>
+      <c r="N35" t="s">
+        <v>396</v>
+      </c>
+      <c r="O35">
+        <v>-1</v>
+      </c>
+      <c r="P35">
+        <v>-1</v>
+      </c>
+      <c r="Q35">
+        <v>20200430</v>
+      </c>
+      <c r="R35" t="s">
+        <v>397</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>-1</v>
+      </c>
+      <c r="U35">
+        <v>20200430</v>
+      </c>
+      <c r="V35" t="s">
+        <v>398</v>
+      </c>
+      <c r="W35">
+        <v>2</v>
+      </c>
+      <c r="X35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20200501</v>
+      </c>
+      <c r="B36" t="s">
+        <v>393</v>
+      </c>
+      <c r="C36">
+        <v>-1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>20200501</v>
+      </c>
+      <c r="F36" t="s">
+        <v>394</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>20200501</v>
+      </c>
+      <c r="J36" t="s">
+        <v>395</v>
+      </c>
+      <c r="K36">
+        <v>-1</v>
+      </c>
+      <c r="L36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>20200501</v>
+      </c>
+      <c r="N36" t="s">
+        <v>396</v>
+      </c>
+      <c r="O36">
+        <v>-1</v>
+      </c>
+      <c r="P36">
+        <v>-1</v>
+      </c>
+      <c r="Q36">
+        <v>20200501</v>
+      </c>
+      <c r="R36" t="s">
+        <v>397</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <v>20200501</v>
+      </c>
+      <c r="V36" t="s">
+        <v>398</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>20200504</v>
+      </c>
+      <c r="B37" t="s">
+        <v>393</v>
+      </c>
+      <c r="C37">
+        <v>-1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>20200504</v>
+      </c>
+      <c r="F37" t="s">
+        <v>394</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>20200504</v>
+      </c>
+      <c r="J37" t="s">
+        <v>395</v>
+      </c>
+      <c r="K37">
+        <v>-2</v>
+      </c>
+      <c r="L37">
+        <v>-1</v>
+      </c>
+      <c r="M37">
+        <v>20200504</v>
+      </c>
+      <c r="N37" t="s">
+        <v>396</v>
+      </c>
+      <c r="O37">
+        <v>-1</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>20200504</v>
+      </c>
+      <c r="R37" t="s">
+        <v>397</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>20200504</v>
+      </c>
+      <c r="V37" t="s">
+        <v>398</v>
+      </c>
+      <c r="W37">
+        <v>-1</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>20200505</v>
+      </c>
+      <c r="B38" t="s">
+        <v>393</v>
+      </c>
+      <c r="C38">
+        <v>-1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>20200505</v>
+      </c>
+      <c r="F38" t="s">
+        <v>394</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>-1</v>
+      </c>
+      <c r="I38">
+        <v>20200505</v>
+      </c>
+      <c r="J38" t="s">
+        <v>395</v>
+      </c>
+      <c r="K38">
+        <v>-2</v>
+      </c>
+      <c r="L38">
+        <v>-1</v>
+      </c>
+      <c r="M38">
+        <v>20200505</v>
+      </c>
+      <c r="N38" t="s">
+        <v>396</v>
+      </c>
+      <c r="O38">
+        <v>-2</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <v>20200505</v>
+      </c>
+      <c r="R38" t="s">
+        <v>397</v>
+      </c>
+      <c r="S38">
+        <v>2</v>
+      </c>
+      <c r="T38">
+        <v>-2</v>
+      </c>
+      <c r="U38">
+        <v>20200505</v>
+      </c>
+      <c r="V38" t="s">
+        <v>398</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>20200506</v>
+      </c>
+      <c r="B39" t="s">
+        <v>393</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>20200506</v>
+      </c>
+      <c r="F39" t="s">
+        <v>394</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>20200506</v>
+      </c>
+      <c r="J39" t="s">
+        <v>395</v>
+      </c>
+      <c r="K39">
+        <v>-2</v>
+      </c>
+      <c r="L39">
+        <v>-1</v>
+      </c>
+      <c r="M39">
+        <v>20200506</v>
+      </c>
+      <c r="N39" t="s">
+        <v>396</v>
+      </c>
+      <c r="O39">
+        <v>-1</v>
+      </c>
+      <c r="P39">
+        <v>-1</v>
+      </c>
+      <c r="Q39">
+        <v>20200506</v>
+      </c>
+      <c r="R39" t="s">
+        <v>397</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+      <c r="T39">
+        <v>-1</v>
+      </c>
+      <c r="U39">
+        <v>20200506</v>
+      </c>
+      <c r="V39" t="s">
+        <v>398</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>20200507</v>
+      </c>
+      <c r="B40" t="s">
+        <v>393</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>-1</v>
+      </c>
+      <c r="E40">
+        <v>20200507</v>
+      </c>
+      <c r="F40" t="s">
+        <v>394</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>20200507</v>
+      </c>
+      <c r="J40" t="s">
+        <v>395</v>
+      </c>
+      <c r="K40">
+        <v>-2</v>
+      </c>
+      <c r="L40">
+        <v>-1</v>
+      </c>
+      <c r="M40">
+        <v>20200507</v>
+      </c>
+      <c r="N40" t="s">
+        <v>396</v>
+      </c>
+      <c r="O40">
+        <v>-1</v>
+      </c>
+      <c r="P40">
+        <v>-1</v>
+      </c>
+      <c r="Q40">
+        <v>20200507</v>
+      </c>
+      <c r="R40" t="s">
+        <v>397</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>20200507</v>
+      </c>
+      <c r="V40" t="s">
+        <v>398</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20200508</v>
+      </c>
+      <c r="B41" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41">
+        <v>-1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>20200508</v>
+      </c>
+      <c r="F41" t="s">
+        <v>394</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>20200508</v>
+      </c>
+      <c r="J41" t="s">
+        <v>395</v>
+      </c>
+      <c r="K41">
+        <v>-2</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>20200508</v>
+      </c>
+      <c r="N41" t="s">
+        <v>396</v>
+      </c>
+      <c r="O41">
+        <v>-1</v>
+      </c>
+      <c r="P41">
+        <v>-1</v>
+      </c>
+      <c r="Q41">
+        <v>20200508</v>
+      </c>
+      <c r="R41" t="s">
+        <v>397</v>
+      </c>
+      <c r="S41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>20200508</v>
+      </c>
+      <c r="V41" t="s">
+        <v>398</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>AVERAGE(C2:C41)</f>
+        <v>-1</v>
+      </c>
+      <c r="D42">
+        <f>AVERAGE(D2:D41)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G42">
+        <f>AVERAGE(G2:G41)</f>
+        <v>-0.05</v>
+      </c>
+      <c r="H42">
+        <f>AVERAGE(H2:H41)</f>
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="K42">
+        <f>AVERAGE(K2:K41)</f>
+        <v>-1.8</v>
+      </c>
+      <c r="L42">
+        <f>AVERAGE(L2:L41)</f>
+        <v>-1.7749999999999999</v>
+      </c>
+      <c r="O42">
+        <f>AVERAGE(O2:O41)</f>
+        <v>-1.2</v>
+      </c>
+      <c r="P42">
+        <f>AVERAGE(P2:P41)</f>
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="S42">
+        <f>AVERAGE(S2:S41)</f>
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="T42">
+        <f>AVERAGE(T2:T41)</f>
+        <v>-0.3</v>
+      </c>
+      <c r="W42">
+        <f>AVERAGE(W2:W41)</f>
+        <v>0.9</v>
+      </c>
+      <c r="X42">
+        <f>AVERAGE(X2:X41)</f>
+        <v>-0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D114"/>
   <sheetViews>
@@ -14266,6 +17334,866 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BE5"/>
+  <sheetViews>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AR7" sqref="AR7:AS7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>43906</v>
+      </c>
+      <c r="C1" s="2">
+        <v>43907</v>
+      </c>
+      <c r="D1" s="2">
+        <v>43908</v>
+      </c>
+      <c r="E1" s="2">
+        <v>43909</v>
+      </c>
+      <c r="F1" s="2">
+        <v>43910</v>
+      </c>
+      <c r="G1" s="2">
+        <v>43911</v>
+      </c>
+      <c r="H1" s="2">
+        <v>43912</v>
+      </c>
+      <c r="I1" s="2">
+        <v>43913</v>
+      </c>
+      <c r="J1" s="2">
+        <v>43914</v>
+      </c>
+      <c r="K1" s="2">
+        <v>43915</v>
+      </c>
+      <c r="L1" s="2">
+        <v>43916</v>
+      </c>
+      <c r="M1" s="2">
+        <v>43917</v>
+      </c>
+      <c r="N1" s="2">
+        <v>43918</v>
+      </c>
+      <c r="O1" s="2">
+        <v>43919</v>
+      </c>
+      <c r="P1" s="2">
+        <v>43920</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>43921</v>
+      </c>
+      <c r="R1" s="2">
+        <v>43922</v>
+      </c>
+      <c r="S1" s="2">
+        <v>43923</v>
+      </c>
+      <c r="T1" s="2">
+        <v>43924</v>
+      </c>
+      <c r="U1" s="2">
+        <v>43925</v>
+      </c>
+      <c r="V1" s="2">
+        <v>43926</v>
+      </c>
+      <c r="W1" s="2">
+        <v>43927</v>
+      </c>
+      <c r="X1" s="2">
+        <v>43928</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>43929</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>43930</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>43931</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>43932</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>43933</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>43934</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>43935</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>43936</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>43937</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>43938</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>43939</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>43940</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>43941</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>43942</v>
+      </c>
+      <c r="AM1" s="2">
+        <v>43943</v>
+      </c>
+      <c r="AN1" s="2">
+        <v>43944</v>
+      </c>
+      <c r="AO1" s="2">
+        <v>43945</v>
+      </c>
+      <c r="AP1" s="2">
+        <v>43946</v>
+      </c>
+      <c r="AQ1" s="2">
+        <v>43947</v>
+      </c>
+      <c r="AR1" s="2">
+        <v>43948</v>
+      </c>
+      <c r="AS1" s="2">
+        <v>43949</v>
+      </c>
+      <c r="AT1" s="2">
+        <v>43950</v>
+      </c>
+      <c r="AU1" s="2">
+        <v>43951</v>
+      </c>
+      <c r="AV1" s="2">
+        <v>43952</v>
+      </c>
+      <c r="AW1" s="2">
+        <v>43953</v>
+      </c>
+      <c r="AX1" s="2">
+        <v>43954</v>
+      </c>
+      <c r="AY1" s="2">
+        <v>43955</v>
+      </c>
+      <c r="AZ1" s="2">
+        <v>43956</v>
+      </c>
+      <c r="BA1" s="2">
+        <v>43957</v>
+      </c>
+      <c r="BB1" s="2">
+        <v>43958</v>
+      </c>
+      <c r="BC1" s="2">
+        <v>43959</v>
+      </c>
+      <c r="BD1" s="2">
+        <v>43960</v>
+      </c>
+      <c r="BE1" s="2">
+        <v>43961</v>
+      </c>
+    </row>
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2">
+        <v>0.51877714199672098</v>
+      </c>
+      <c r="C2">
+        <v>0.58604294682272196</v>
+      </c>
+      <c r="D2">
+        <v>0.58554710498468399</v>
+      </c>
+      <c r="E2">
+        <v>0.58045837319761895</v>
+      </c>
+      <c r="F2">
+        <v>0.58456302302560204</v>
+      </c>
+      <c r="G2">
+        <v>0.47637227031923102</v>
+      </c>
+      <c r="H2">
+        <v>0.54006811750051698</v>
+      </c>
+      <c r="I2">
+        <v>0.63297628608867096</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.68038189041817099</v>
+      </c>
+      <c r="K2">
+        <v>0.66348030669511204</v>
+      </c>
+      <c r="L2">
+        <v>0.65062437478040103</v>
+      </c>
+      <c r="M2">
+        <v>0.58445668562025999</v>
+      </c>
+      <c r="N2">
+        <v>0.54626366174705299</v>
+      </c>
+      <c r="O2">
+        <v>0.58589800564161798</v>
+      </c>
+      <c r="P2">
+        <v>0.65037441715333799</v>
+      </c>
+      <c r="Q2">
+        <v>0.65990408105230203</v>
+      </c>
+      <c r="R2">
+        <v>0.66128589397651005</v>
+      </c>
+      <c r="S2">
+        <v>0.64411973215234397</v>
+      </c>
+      <c r="T2">
+        <v>0.59769043122729104</v>
+      </c>
+      <c r="U2">
+        <v>0.56735739010837904</v>
+      </c>
+      <c r="V2">
+        <v>0.62888494404891004</v>
+      </c>
+      <c r="W2">
+        <v>0.64762987104729197</v>
+      </c>
+      <c r="X2">
+        <v>0.68589430390542905</v>
+      </c>
+      <c r="Y2">
+        <v>0.65225154709559796</v>
+      </c>
+      <c r="Z2">
+        <v>0.66832842974258</v>
+      </c>
+      <c r="AA2">
+        <v>0.59224016065720697</v>
+      </c>
+      <c r="AB2">
+        <v>0.55357283181626205</v>
+      </c>
+      <c r="AC2">
+        <v>0.62052691777188196</v>
+      </c>
+      <c r="AD2">
+        <v>0.65098126675736701</v>
+      </c>
+      <c r="AE2">
+        <v>0.674377577689667</v>
+      </c>
+      <c r="AF2">
+        <v>0.64901996309179599</v>
+      </c>
+      <c r="AG2">
+        <v>0.64485457634150301</v>
+      </c>
+      <c r="AH2">
+        <v>0.56670344605336898</v>
+      </c>
+      <c r="AI2">
+        <v>0.59488576433607698</v>
+      </c>
+      <c r="AJ2">
+        <v>0.61888775009566599</v>
+      </c>
+      <c r="AK2">
+        <v>0.65008751756527505</v>
+      </c>
+      <c r="AL2">
+        <v>0.67305243542423199</v>
+      </c>
+      <c r="AM2">
+        <v>0.64911715802990499</v>
+      </c>
+      <c r="AN2">
+        <v>0.65135157625742302</v>
+      </c>
+      <c r="AO2">
+        <v>0.58946479302810795</v>
+      </c>
+      <c r="AP2">
+        <v>0.583810481418782</v>
+      </c>
+      <c r="AQ2">
+        <v>0.61909450661125198</v>
+      </c>
+      <c r="AR2">
+        <v>0.62235982388427202</v>
+      </c>
+      <c r="AS2">
+        <v>0.65549077902901498</v>
+      </c>
+      <c r="AT2">
+        <v>0.65479720889242299</v>
+      </c>
+      <c r="AU2">
+        <v>0.64728508990324896</v>
+      </c>
+      <c r="AV2">
+        <v>0.56756639691503696</v>
+      </c>
+      <c r="AW2">
+        <v>0.55943008766925895</v>
+      </c>
+      <c r="AX2">
+        <v>0.59625624654800002</v>
+      </c>
+      <c r="AY2">
+        <v>0.63848690605768199</v>
+      </c>
+      <c r="AZ2">
+        <v>0.63320715250395199</v>
+      </c>
+      <c r="BA2">
+        <v>0.61378534887356995</v>
+      </c>
+      <c r="BB2">
+        <v>0.618943999993817</v>
+      </c>
+      <c r="BC2">
+        <v>0.57598178148840595</v>
+      </c>
+      <c r="BD2">
+        <v>0.56360122539038804</v>
+      </c>
+      <c r="BE2">
+        <v>0.58120891193178503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.147823149014707</v>
+      </c>
+      <c r="C3">
+        <v>0.20182404972118101</v>
+      </c>
+      <c r="D3">
+        <v>0.194842652464641</v>
+      </c>
+      <c r="E3">
+        <v>0.203044778428185</v>
+      </c>
+      <c r="F3">
+        <v>0.16558583973448099</v>
+      </c>
+      <c r="G3">
+        <v>0.17519233386598701</v>
+      </c>
+      <c r="H3">
+        <v>0.193908373957205</v>
+      </c>
+      <c r="I3">
+        <v>0.17939598219300901</v>
+      </c>
+      <c r="J3">
+        <v>0.18897631191939801</v>
+      </c>
+      <c r="K3">
+        <v>0.20979115312107099</v>
+      </c>
+      <c r="L3">
+        <v>0.19585535017962799</v>
+      </c>
+      <c r="M3">
+        <v>0.20178410163991001</v>
+      </c>
+      <c r="N3">
+        <v>0.215192243442933</v>
+      </c>
+      <c r="O3">
+        <v>0.22125099818434199</v>
+      </c>
+      <c r="P3">
+        <v>0.238892371599735</v>
+      </c>
+      <c r="Q3">
+        <v>0.210530536036207</v>
+      </c>
+      <c r="R3">
+        <v>0.20401910421785699</v>
+      </c>
+      <c r="S3">
+        <v>0.203985689855919</v>
+      </c>
+      <c r="T3">
+        <v>0.18760533251761</v>
+      </c>
+      <c r="U3">
+        <v>0.26487237544248798</v>
+      </c>
+      <c r="V3">
+        <v>0.24695816798438699</v>
+      </c>
+      <c r="W3">
+        <v>0.220580083756583</v>
+      </c>
+      <c r="X3">
+        <v>0.22438644042386399</v>
+      </c>
+      <c r="Y3">
+        <v>0.22265719455667299</v>
+      </c>
+      <c r="Z3">
+        <v>0.236620701975185</v>
+      </c>
+      <c r="AA3">
+        <v>0.23326153236043601</v>
+      </c>
+      <c r="AB3">
+        <v>0.26371190954018597</v>
+      </c>
+      <c r="AC3">
+        <v>0.26583073264662499</v>
+      </c>
+      <c r="AD3">
+        <v>0.22252343493849</v>
+      </c>
+      <c r="AE3">
+        <v>0.235670152348573</v>
+      </c>
+      <c r="AF3">
+        <v>0.241529242236345</v>
+      </c>
+      <c r="AG3">
+        <v>0.254634870268451</v>
+      </c>
+      <c r="AH3">
+        <v>0.22088959975366099</v>
+      </c>
+      <c r="AI3">
+        <v>0.28387879970759</v>
+      </c>
+      <c r="AJ3">
+        <v>0.25170337351292998</v>
+      </c>
+      <c r="AK3">
+        <v>0.21251118984971501</v>
+      </c>
+      <c r="AL3">
+        <v>0.23160564810190401</v>
+      </c>
+      <c r="AM3">
+        <v>0.219303718719629</v>
+      </c>
+      <c r="AN3">
+        <v>0.236732055465152</v>
+      </c>
+      <c r="AO3">
+        <v>0.212099138597765</v>
+      </c>
+      <c r="AP3">
+        <v>0.27989394201057999</v>
+      </c>
+      <c r="AQ3">
+        <v>0.239708029005894</v>
+      </c>
+      <c r="AR3">
+        <v>0.249803397147489</v>
+      </c>
+      <c r="AS3">
+        <v>0.23347327636912499</v>
+      </c>
+      <c r="AT3">
+        <v>0.23620149675833499</v>
+      </c>
+      <c r="AU3">
+        <v>0.24018129206043201</v>
+      </c>
+      <c r="AV3">
+        <v>0.205139537453396</v>
+      </c>
+      <c r="AW3">
+        <v>0.271904961702367</v>
+      </c>
+      <c r="AX3">
+        <v>0.25083004238578299</v>
+      </c>
+      <c r="AY3">
+        <v>0.237633832518096</v>
+      </c>
+      <c r="AZ3">
+        <v>0.24329925206890399</v>
+      </c>
+      <c r="BA3">
+        <v>0.19924343572116601</v>
+      </c>
+      <c r="BB3">
+        <v>0.225403722858394</v>
+      </c>
+      <c r="BC3">
+        <v>0.22000767213873601</v>
+      </c>
+      <c r="BD3">
+        <v>0.266832962434498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2.08220622818639</v>
+      </c>
+      <c r="C4">
+        <v>2.7117367684263902</v>
+      </c>
+      <c r="D4">
+        <v>3.0480065043932498</v>
+      </c>
+      <c r="E4">
+        <v>3.3281018337746899</v>
+      </c>
+      <c r="F4">
+        <v>3.2512127262058099</v>
+      </c>
+      <c r="G4">
+        <v>2.9829583654107998</v>
+      </c>
+      <c r="H4">
+        <v>2.9709548379175201</v>
+      </c>
+      <c r="I4">
+        <v>3.8098386942319902</v>
+      </c>
+      <c r="J4">
+        <v>4.1833956504850702</v>
+      </c>
+      <c r="K4">
+        <v>4.3214995094142603</v>
+      </c>
+      <c r="L4">
+        <v>4.3055968796570001</v>
+      </c>
+      <c r="M4">
+        <v>4.2326090042750097</v>
+      </c>
+      <c r="N4">
+        <v>3.7198016306528499</v>
+      </c>
+      <c r="O4">
+        <v>3.3891834613601599</v>
+      </c>
+      <c r="P4">
+        <v>4.0897332472813801</v>
+      </c>
+      <c r="Q4">
+        <v>4.4894081613528396</v>
+      </c>
+      <c r="R4">
+        <v>4.6927733896630999</v>
+      </c>
+      <c r="S4">
+        <v>4.8264057043208597</v>
+      </c>
+      <c r="T4">
+        <v>4.6445814413100397</v>
+      </c>
+      <c r="U4">
+        <v>3.9487254296686198</v>
+      </c>
+      <c r="V4">
+        <v>3.9677867802281201</v>
+      </c>
+      <c r="W4">
+        <v>4.8788008871518098</v>
+      </c>
+      <c r="X4">
+        <v>5.1060775141123598</v>
+      </c>
+      <c r="Y4">
+        <v>5.2382435902289597</v>
+      </c>
+      <c r="Z4">
+        <v>5.4458289568428304</v>
+      </c>
+      <c r="AA4">
+        <v>5.20017847304561</v>
+      </c>
+      <c r="AB4">
+        <v>4.4174936500776401</v>
+      </c>
+      <c r="AC4">
+        <v>4.6952994897446496</v>
+      </c>
+      <c r="AD4">
+        <v>5.3948876334519298</v>
+      </c>
+      <c r="AE4">
+        <v>5.5505770008209101</v>
+      </c>
+      <c r="AF4">
+        <v>5.9009764079310303</v>
+      </c>
+      <c r="AG4">
+        <v>5.8329324784449899</v>
+      </c>
+      <c r="AH4">
+        <v>5.5671580520742099</v>
+      </c>
+      <c r="AI4">
+        <v>4.8116750223036604</v>
+      </c>
+      <c r="AJ4">
+        <v>4.5790667019948597</v>
+      </c>
+      <c r="AK4">
+        <v>5.1981725884593502</v>
+      </c>
+      <c r="AL4">
+        <v>5.8145829805467404</v>
+      </c>
+      <c r="AM4" s="6">
+        <v>6.0121168998477801</v>
+      </c>
+      <c r="AN4">
+        <v>5.9300335867198797</v>
+      </c>
+      <c r="AO4">
+        <v>5.8612936344147997</v>
+      </c>
+      <c r="AP4">
+        <v>4.8287623432376598</v>
+      </c>
+      <c r="AQ4">
+        <v>4.86818581792462</v>
+      </c>
+      <c r="AR4">
+        <v>5.8341120273059603</v>
+      </c>
+      <c r="AS4">
+        <v>5.9314730803847304</v>
+      </c>
+      <c r="AT4">
+        <v>5.7447467554326002</v>
+      </c>
+      <c r="AU4" s="5">
+        <v>6.1037650836254098</v>
+      </c>
+      <c r="AV4">
+        <v>5.3310233646314398</v>
+      </c>
+      <c r="AW4">
+        <v>4.5735422132923196</v>
+      </c>
+      <c r="AX4">
+        <v>4.3972287267054897</v>
+      </c>
+      <c r="AY4">
+        <v>5.0425757791356398</v>
+      </c>
+      <c r="AZ4">
+        <v>5.4017567982475203</v>
+      </c>
+      <c r="BA4">
+        <v>5.5715497414625901</v>
+      </c>
+      <c r="BB4">
+        <v>5.2882839058876998</v>
+      </c>
+      <c r="BC4">
+        <v>5.1827396156364101</v>
+      </c>
+      <c r="BD4">
+        <v>4.3645646087449599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.62940291429178097</v>
+      </c>
+      <c r="C5">
+        <v>1.3620930422317299</v>
+      </c>
+      <c r="D5">
+        <v>1.8808588551230201</v>
+      </c>
+      <c r="E5">
+        <v>2.0064016106262299</v>
+      </c>
+      <c r="F5">
+        <v>1.7809616394515899</v>
+      </c>
+      <c r="G5">
+        <v>1.3861208985728499</v>
+      </c>
+      <c r="H5">
+        <v>1.6257045220329001</v>
+      </c>
+      <c r="I5">
+        <v>2.26328970455527</v>
+      </c>
+      <c r="J5">
+        <v>2.9250229144648299</v>
+      </c>
+      <c r="K5">
+        <v>2.8665832366028701</v>
+      </c>
+      <c r="L5">
+        <v>2.89996603377769</v>
+      </c>
+      <c r="M5">
+        <v>3.26102900836195</v>
+      </c>
+      <c r="N5">
+        <v>1.94393927272496</v>
+      </c>
+      <c r="O5">
+        <v>2.0178013580576502</v>
+      </c>
+      <c r="P5">
+        <v>3.01912439163624</v>
+      </c>
+      <c r="Q5">
+        <v>3.53646145407376</v>
+      </c>
+      <c r="R5">
+        <v>4.2983951461524104</v>
+      </c>
+      <c r="S5">
+        <v>4.3192534312196198</v>
+      </c>
+      <c r="T5">
+        <v>4.4119349154516101</v>
+      </c>
+      <c r="U5">
+        <v>2.1286379383664298</v>
+      </c>
+      <c r="V5">
+        <v>3.4003740264297102</v>
+      </c>
+      <c r="W5">
+        <v>3.8444692440944399</v>
+      </c>
+      <c r="X5">
+        <v>3.8176435767132801</v>
+      </c>
+      <c r="Y5">
+        <v>4.80728563425202</v>
+      </c>
+      <c r="Z5">
+        <v>4.1870503804375003</v>
+      </c>
+      <c r="AA5">
+        <v>4.6476316232695796</v>
+      </c>
+      <c r="AB5">
+        <v>3.6750786650477698</v>
+      </c>
+      <c r="AC5">
+        <v>4.5156489103153898</v>
+      </c>
+      <c r="AD5">
+        <v>4.46350460996943</v>
+      </c>
+      <c r="AE5">
+        <v>5.4196700272672702</v>
+      </c>
+      <c r="AF5">
+        <v>6.5131937582413499</v>
+      </c>
+      <c r="AG5">
+        <v>5.6325601159289302</v>
+      </c>
+      <c r="AH5">
+        <v>6.0300403469420596</v>
+      </c>
+      <c r="AI5">
+        <v>4.7390089357244003</v>
+      </c>
+      <c r="AJ5">
+        <v>5.5752128870645699</v>
+      </c>
+      <c r="AK5">
+        <v>4.9106831843650802</v>
+      </c>
+      <c r="AL5">
+        <v>6.3715082204107603</v>
+      </c>
+      <c r="AM5">
+        <v>6.3725039980163398</v>
+      </c>
+      <c r="AN5">
+        <v>6.5501946016083101</v>
+      </c>
+      <c r="AO5">
+        <v>6.5526924026751701</v>
+      </c>
+      <c r="AP5">
+        <v>5.1013549472704796</v>
+      </c>
+      <c r="AQ5">
+        <v>6.0755290629185197</v>
+      </c>
+      <c r="AR5">
+        <v>7.4873573976545504</v>
+      </c>
+      <c r="AS5">
+        <v>8.1577196233869405</v>
+      </c>
+      <c r="AT5">
+        <v>5.9949753728455599</v>
+      </c>
+      <c r="AU5">
+        <v>7.2935728375427598</v>
+      </c>
+      <c r="AV5">
+        <v>5.8699563078837897</v>
+      </c>
+      <c r="AW5">
+        <v>5.2403188047221203</v>
+      </c>
+      <c r="AX5">
+        <v>5.52977233706146</v>
+      </c>
+      <c r="AY5">
+        <v>5.2063659592986298</v>
+      </c>
+      <c r="AZ5">
+        <v>5.94681045036518</v>
+      </c>
+      <c r="BA5">
+        <v>6.2628856179282799</v>
+      </c>
+      <c r="BB5">
+        <v>5.2937549565272297</v>
+      </c>
+      <c r="BC5">
+        <v>5.1088916957054797</v>
+      </c>
+      <c r="BD5">
+        <v>4.2175184014033098</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update new conclusions about Google Search index and fix some error. Update draft. Send it to HJM
</commit_message>
<xml_diff>
--- a/doc/excels/temporal.xlsx
+++ b/doc/excels/temporal.xlsx
@@ -11177,7 +11177,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12697,10 +12697,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X42"/>
+  <dimension ref="A2:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="K13" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15716,6 +15716,32 @@
       <c r="X42">
         <f>AVERAGE(X2:X41)</f>
         <v>-0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f>D42-C42</f>
+        <v>1.25</v>
+      </c>
+      <c r="G43">
+        <f>H42-G42</f>
+        <v>-0.5</v>
+      </c>
+      <c r="K43">
+        <f>L42-K42</f>
+        <v>2.5000000000000133E-2</v>
+      </c>
+      <c r="O43">
+        <f>P42-O42</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="S43">
+        <f>T42-S42</f>
+        <v>-1.5250000000000001</v>
+      </c>
+      <c r="W43">
+        <f>X42-W42</f>
+        <v>-1.4500000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>